<commit_message>
Encodage des swords dans un fichier xml
</commit_message>
<xml_diff>
--- a/Documentation/WeaponTypes.xlsx
+++ b/Documentation/WeaponTypes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxad\Documents\git_projects\LC_Unity\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity_Projects\LC_Unity\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C9EEC27-1991-435B-92EB-1EFE5FD08842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC030377-FD88-4343-8635-C6B3C85FE279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AF0181E3-6649-48B0-8903-A18ED6172CFD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
   <si>
     <t>Sword</t>
   </si>
@@ -173,6 +173,12 @@
 - Strikes in a 150° cone in front of the user
 - Damage is based off both Strength and Magic
 - Has Health and Mana drain</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Magical</t>
   </si>
 </sst>
 </file>
@@ -554,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D266849-7905-4F0E-8747-E73D82D0397A}">
-  <dimension ref="B1:F15"/>
+  <dimension ref="B1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +571,7 @@
     <col min="6" max="6" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
@@ -581,8 +587,23 @@
       <c r="F1" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -598,8 +619,27 @@
       <c r="F2" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>32</v>
+      </c>
+      <c r="J2">
+        <f>G2+G3+G4+G5+G6+G7+G8+G9+G14+G15</f>
+        <v>168</v>
+      </c>
+      <c r="K2">
+        <f>G13+G12+G11+G10</f>
+        <v>57</v>
+      </c>
+      <c r="M2">
+        <f>G2+G3+G4+G5+G6+G7+G11+G12+G13</f>
+        <v>152</v>
+      </c>
+      <c r="N2">
+        <f>G8+G9+G10+G14+G15</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" ht="90" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -615,8 +655,11 @@
       <c r="F3" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -632,8 +675,11 @@
       <c r="F4" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="90" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -649,8 +695,11 @@
       <c r="F5" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -666,8 +715,11 @@
       <c r="F6" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -683,8 +735,11 @@
       <c r="F7" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -700,8 +755,11 @@
       <c r="F8" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -717,8 +775,11 @@
       <c r="F9" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -734,8 +795,11 @@
       <c r="F10" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -751,8 +815,11 @@
       <c r="F11" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="90" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -768,8 +835,11 @@
       <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="60" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -785,8 +855,11 @@
       <c r="F13" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>13</v>
       </c>
@@ -802,8 +875,11 @@
       <c r="F14" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="90" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>14</v>
       </c>
@@ -818,6 +894,15 @@
       </c>
       <c r="F15" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="G15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <f>SUM(G2:G15)</f>
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>